<commit_message>
build na git pull
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/zorgwekkende_stof/zorgwekkende_stof.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/zorgwekkende_stof/zorgwekkende_stof.xlsx
@@ -689,7 +689,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/AFDRCEOKCOUICI-UHFFFAOYSA-N</v>
       </c>
       <c r="B7" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C7" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -736,7 +736,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/ALEROMXYYSQFLX-UHFFFAOYSA-N</v>
       </c>
       <c r="B8" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C8" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -783,7 +783,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/ATBAMAFKBVZNFJ-UHFFFAOYSA-N</v>
       </c>
       <c r="B9" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C9" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -830,7 +830,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/BBEAQIROQSPTKN-UHFFFAOYSA-N</v>
       </c>
       <c r="B10" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C10" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -877,7 +877,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/BFCFYVKQTRLZHA-UHFFFAOYSA-N</v>
       </c>
       <c r="B11" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C11" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -924,7 +924,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/BRLQWZUYTZBJKN-UHFFFAOYSA-N</v>
       </c>
       <c r="B12" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C12" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -971,7 +971,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/BZHJMEDXRYGGRV-UHFFFAOYSA-N</v>
       </c>
       <c r="B13" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C13" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1018,7 +1018,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/BZLVMXJERCGZMT-UHFFFAOYSA-N</v>
       </c>
       <c r="B14" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C14" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1065,7 +1065,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/CFXQEHVMCRXUSD-UHFFFAOYSA-N</v>
       </c>
       <c r="B15" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C15" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1112,7 +1112,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/CSEBNABAWMZWIF-UHFFFAOYSA-N</v>
       </c>
       <c r="B16" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C16" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1159,7 +1159,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/CWRYPZZKDGJXCA-UHFFFAOYSA-N</v>
       </c>
       <c r="B17" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C17" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1206,7 +1206,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/CXGONMQFMIYUJR-UHFFFAOYSA-N</v>
       </c>
       <c r="B18" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C18" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1253,7 +1253,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/CXNVOWPRHWWCQR-UHFFFAOYSA-N</v>
       </c>
       <c r="B19" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C19" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1300,7 +1300,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/CYTYCFOTNPOANT-UHFFFAOYSA-N</v>
       </c>
       <c r="B20" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C20" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1347,7 +1347,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/CZGCEKJOLUNIFY-UHFFFAOYSA-N</v>
       </c>
       <c r="B21" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C21" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1394,7 +1394,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/DDBMQDADIHOWIC-UHFFFAOYSA-N</v>
       </c>
       <c r="B22" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C22" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1441,7 +1441,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/DEWLEGDTCGBNGU-UHFFFAOYSA-N</v>
       </c>
       <c r="B23" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C23" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1488,7 +1488,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/DKGAVHZHDRPRBM-UHFFFAOYSA-N</v>
       </c>
       <c r="B24" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C24" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1535,7 +1535,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/DOIRQSBPFJWKBE-UHFFFAOYSA-N</v>
       </c>
       <c r="B25" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C25" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1582,7 +1582,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/DXBHBZVCASKNBY-UHFFFAOYSA-N</v>
       </c>
       <c r="B26" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C26" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1629,7 +1629,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/FOIBFBMSLDGNHL-UHFFFAOYSA-N</v>
       </c>
       <c r="B27" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C27" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1676,7 +1676,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/FSAVDKDHPDSCTO-WQLSENKSSA-N</v>
       </c>
       <c r="B28" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C28" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1723,7 +1723,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/FSPZPQQWDODWAU-UHFFFAOYSA-N</v>
       </c>
       <c r="B29" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C29" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1770,7 +1770,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/GOOHAUXETOMSMM-UHFFFAOYSA-N</v>
       </c>
       <c r="B30" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C30" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1817,7 +1817,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/GUTLYIVDDKVIGB-UHFFFAOYSA-N</v>
       </c>
       <c r="B31" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C31" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1864,7 +1864,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/GVEPBJHOBDJJJI-UHFFFAOYSA-N</v>
       </c>
       <c r="B32" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C32" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1911,7 +1911,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/GYFAGKUZYNFMBN-UHFFFAOYSA-N</v>
       </c>
       <c r="B33" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C33" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -1958,7 +1958,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/HDHLIWCXDDZUFH-UHFFFAOYSA-N</v>
       </c>
       <c r="B34" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C34" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -2005,7 +2005,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/HEDRZPFGACZZDS-UHFFFAOYSA-N</v>
       </c>
       <c r="B35" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C35" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -2052,7 +2052,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/HFACYLZERDEVSX-UHFFFAOYSA-N</v>
       </c>
       <c r="B36" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C36" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -2099,7 +2099,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/HFZWRUODUSTPEG-UHFFFAOYSA-N</v>
       </c>
       <c r="B37" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C37" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -2146,7 +2146,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/HGUFODBRKLSHSI-UHFFFAOYSA-N</v>
       </c>
       <c r="B38" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C38" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/zorgwekkende_stof</v>
@@ -2193,7 +2193,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/HRYZWHHZPQKTII-UHFFFAOYSA-N</v>
       </c>
       <c r="B39" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C39" t="str">
         <v>null</v>
@@ -2240,7 +2240,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/HUWXDEQWWKGHRV-UHFFFAOYSA-N</v>
       </c>
       <c r="B40" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C40" t="str">
         <v>null</v>
@@ -2287,7 +2287,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/IBOFVQJTBBUKMU-UHFFFAOYSA-N</v>
       </c>
       <c r="B41" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C41" t="str">
         <v>null</v>
@@ -2334,7 +2334,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/IISBACLAFKSPIT-UHFFFAOYSA-N</v>
       </c>
       <c r="B42" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C42" t="str">
         <v>null</v>
@@ -2381,7 +2381,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/IPKKHRVROFYTEK-UHFFFAOYSA-N</v>
       </c>
       <c r="B43" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C43" t="str">
         <v>null</v>
@@ -2428,7 +2428,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/IRIAEXORFWYRCZ-UHFFFAOYSA-N</v>
       </c>
       <c r="B44" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C44" t="str">
         <v>null</v>
@@ -2475,7 +2475,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/IROINLKCQGIITA-UHFFFAOYSA-N</v>
       </c>
       <c r="B45" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C45" t="str">
         <v>null</v>
@@ -2522,7 +2522,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/JANBFCARANRIKJ-UHFFFAOYSA-N</v>
       </c>
       <c r="B46" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C46" t="str">
         <v>null</v>
@@ -2569,7 +2569,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/JBIJLHTVPXGSAM-UHFFFAOYSA-N</v>
       </c>
       <c r="B47" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C47" t="str">
         <v>null</v>
@@ -2616,7 +2616,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/JEYJJJXOFWNEHN-UHFFFAOYSA-N</v>
       </c>
       <c r="B48" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C48" t="str">
         <v>null</v>
@@ -2663,7 +2663,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/JGTNAGYHADQMCM-UHFFFAOYSA-N</v>
       </c>
       <c r="B49" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C49" t="str">
         <v>null</v>
@@ -2710,7 +2710,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/JSFITYFUKSFPBZ-UHFFFAOYSA-N</v>
       </c>
       <c r="B50" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C50" t="str">
         <v>null</v>
@@ -2757,7 +2757,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/JVZREVRTMWNFME-UHFFFAOYSA-N</v>
       </c>
       <c r="B51" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C51" t="str">
         <v>null</v>
@@ -2804,7 +2804,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/KAATUXNTWXVJKI-UHFFFAOYSA-N</v>
       </c>
       <c r="B52" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C52" t="str">
         <v>null</v>
@@ -2851,7 +2851,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/KAKZBPTYRLMSJV-UHFFFAOYSA-N</v>
       </c>
       <c r="B53" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C53" t="str">
         <v>null</v>
@@ -2898,7 +2898,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/KCXMKQUNVWSEMD-UHFFFAOYSA-N</v>
       </c>
       <c r="B54" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C54" t="str">
         <v>null</v>
@@ -2945,7 +2945,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/KCXZNSGUUQJJTR-UHFFFAOYSA-N</v>
       </c>
       <c r="B55" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C55" t="str">
         <v>null</v>
@@ -2992,7 +2992,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/KFUSEUYYWQURPO-OWOJBTEDSA-N</v>
       </c>
       <c r="B56" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C56" t="str">
         <v>null</v>
@@ -3039,7 +3039,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/KNKRKFALVUDBJE-UHFFFAOYSA-N</v>
       </c>
       <c r="B57" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C57" t="str">
         <v>null</v>
@@ -3086,7 +3086,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/KSMVNVHUTQZITP-UHFFFAOYSA-N</v>
       </c>
       <c r="B58" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C58" t="str">
         <v>null</v>
@@ -3133,7 +3133,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/LGIRBUBHIWTVCK-UHFFFAOYSA-N</v>
       </c>
       <c r="B59" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C59" t="str">
         <v>null</v>
@@ -3180,7 +3180,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/LGXVIGDEPROXKC-UHFFFAOYSA-N</v>
       </c>
       <c r="B60" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C60" t="str">
         <v>null</v>
@@ -3227,7 +3227,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/LHRCREOYAASXPZ-UHFFFAOYSA-N</v>
       </c>
       <c r="B61" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C61" t="str">
         <v>null</v>
@@ -3274,7 +3274,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/LVDGGZAZAYHXEY-UHFFFAOYSA-N</v>
       </c>
       <c r="B62" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C62" t="str">
         <v>null</v>
@@ -3321,7 +3321,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/LVYBAQIVPKCOEE-UHFFFAOYSA-N</v>
       </c>
       <c r="B63" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C63" t="str">
         <v>null</v>
@@ -3368,7 +3368,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/MGWAVDBGNNKXQV-UHFFFAOYSA-N</v>
       </c>
       <c r="B64" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C64" t="str">
         <v>null</v>
@@ -3415,7 +3415,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/MQIUGAXCHLFZKX-UHFFFAOYSA-N</v>
       </c>
       <c r="B65" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C65" t="str">
         <v>null</v>
@@ -3462,7 +3462,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/MVPPADPHJFYWMZ-UHFFFAOYSA-N</v>
       </c>
       <c r="B66" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C66" t="str">
         <v>null</v>
@@ -3509,7 +3509,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/MWPLVEDNUUSJAV-UHFFFAOYSA-N</v>
       </c>
       <c r="B67" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C67" t="str">
         <v>null</v>
@@ -3556,7 +3556,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/MXWJVTOOROXGIU-UHFFFAOYSA-N</v>
       </c>
       <c r="B68" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C68" t="str">
         <v>null</v>
@@ -3603,7 +3603,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/NLHHRLWOUZZQLW-UHFFFAOYSA-N</v>
       </c>
       <c r="B69" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C69" t="str">
         <v>null</v>
@@ -3650,7 +3650,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/NOWKCMXCCJGMRR-UHFFFAOYSA-N</v>
       </c>
       <c r="B70" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C70" t="str">
         <v>null</v>
@@ -3697,7 +3697,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/OAKJQQAXSVQMHS-UHFFFAOYSA-N</v>
       </c>
       <c r="B71" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C71" t="str">
         <v>null</v>
@@ -3744,7 +3744,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/OCJBOOLMMGQPQU-UHFFFAOYSA-N</v>
       </c>
       <c r="B72" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C72" t="str">
         <v>null</v>
@@ -3791,7 +3791,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/ODCWYMIRDDJXKW-UHFFFAOYSA-N</v>
       </c>
       <c r="B73" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C73" t="str">
         <v>null</v>
@@ -3838,7 +3838,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/OEBRKCOSUFCWJD-UHFFFAOYSA-N</v>
       </c>
       <c r="B74" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C74" t="str">
         <v>null</v>
@@ -3885,7 +3885,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/OGBQILNBLMPPDP-UHFFFAOYSA-N</v>
       </c>
       <c r="B75" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C75" t="str">
         <v>null</v>
@@ -3932,7 +3932,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/PAAZPARNPHGIKF-UHFFFAOYSA-N</v>
       </c>
       <c r="B76" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C76" t="str">
         <v>null</v>
@@ -3979,7 +3979,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/PBGKNXWGYQPUJK-UHFFFAOYSA-N</v>
       </c>
       <c r="B77" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C77" t="str">
         <v>null</v>
@@ -4026,7 +4026,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/PCIUEQPBYFRTEM-UHFFFAOYSA-N</v>
       </c>
       <c r="B78" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C78" t="str">
         <v>null</v>
@@ -4073,7 +4073,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/PNPCRKVUWYDDST-UHFFFAOYSA-N</v>
       </c>
       <c r="B79" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C79" t="str">
         <v>null</v>
@@ -4120,7 +4120,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/PUIYMUZLKQOUOZ-UHFFFAOYSA-N</v>
       </c>
       <c r="B80" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C80" t="str">
         <v>null</v>
@@ -4167,7 +4167,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/PXBRQCKWGAHEHS-UHFFFAOYSA-N</v>
       </c>
       <c r="B81" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C81" t="str">
         <v>null</v>
@@ -4214,7 +4214,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/PXUULQAPEKKVAH-UHFFFAOYSA-N</v>
       </c>
       <c r="B82" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C82" t="str">
         <v>null</v>
@@ -4261,7 +4261,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/PYUSJFJVDVSXIU-UHFFFAOYSA-N</v>
       </c>
       <c r="B83" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C83" t="str">
         <v>null</v>
@@ -4308,7 +4308,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/QPFMBZIOSGYJDE-UHFFFAOYSA-N</v>
       </c>
       <c r="B84" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C84" t="str">
         <v>null</v>
@@ -4355,7 +4355,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/QSHDDOUJBYECFT-UHFFFAOYSA-N</v>
       </c>
       <c r="B85" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C85" t="str">
         <v>null</v>
@@ -4402,7 +4402,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/QSNSCYSYFYORTR-UHFFFAOYSA-N</v>
       </c>
       <c r="B86" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C86" t="str">
         <v>null</v>
@@ -4449,7 +4449,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/QVLAWKAXOMEXPM-UHFFFAOYSA-N</v>
       </c>
       <c r="B87" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C87" t="str">
         <v>null</v>
@@ -4496,7 +4496,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/QZHDEAJFRJCDMF-UHFFFAOYSA-N</v>
       </c>
       <c r="B88" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C88" t="str">
         <v>null</v>
@@ -4543,7 +4543,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/RFFLAFLAYFXFSW-UHFFFAOYSA-N</v>
       </c>
       <c r="B89" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C89" t="str">
         <v>null</v>
@@ -4590,7 +4590,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/RHIROFAGUQOFLU-UHFFFAOYSA-N</v>
       </c>
       <c r="B90" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C90" t="str">
         <v>null</v>
@@ -4637,7 +4637,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/RKELNIPLHQEBJO-UHFFFAOYSA-N</v>
       </c>
       <c r="B91" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C91" t="str">
         <v>null</v>
@@ -4684,7 +4684,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/RNVCVTLRINQCPJ-UHFFFAOYSA-N</v>
       </c>
       <c r="B92" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C92" t="str">
         <v>null</v>
@@ -4731,7 +4731,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/RQNWIZPPADIBDY-UHFFFAOYSA-N</v>
       </c>
       <c r="B93" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C93" t="str">
         <v>null</v>
@@ -4778,7 +4778,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/RUDINRUXCKIXAJ-UHFFFAOYSA-N</v>
       </c>
       <c r="B94" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C94" t="str">
         <v>null</v>
@@ -4825,7 +4825,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/RWGFKTVRMDUZSP-UHFFFAOYSA-N</v>
       </c>
       <c r="B95" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C95" t="str">
         <v>null</v>
@@ -4872,7 +4872,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/RYHBNJHYFVUHQT-UHFFFAOYSA-N</v>
       </c>
       <c r="B96" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C96" t="str">
         <v>null</v>
@@ -4919,7 +4919,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/SBMIVUVRFPGOEB-UHFFFAOYSA-N</v>
       </c>
       <c r="B97" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C97" t="str">
         <v>null</v>
@@ -4966,7 +4966,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/SBPBAQFWLVIOKP-UHFFFAOYSA-N</v>
       </c>
       <c r="B98" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C98" t="str">
         <v>null</v>
@@ -5013,7 +5013,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/SDYWXFYBZPNOFX-UHFFFAOYSA-N</v>
       </c>
       <c r="B99" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C99" t="str">
         <v>null</v>
@@ -5060,7 +5060,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/SECXISVLQFMRJM-UHFFFAOYSA-N</v>
       </c>
       <c r="B100" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C100" t="str">
         <v>null</v>
@@ -5107,7 +5107,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/SIDINRCMMRKXGQ-UHFFFAOYSA-N</v>
       </c>
       <c r="B101" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C101" t="str">
         <v>null</v>
@@ -5154,7 +5154,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/SUSRORUBZHMPCO-UHFFFAOYSA-N</v>
       </c>
       <c r="B102" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C102" t="str">
         <v>null</v>
@@ -5201,7 +5201,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/UBOXGVDOUJQMTN-UHFFFAOYSA-N</v>
       </c>
       <c r="B103" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C103" t="str">
         <v>null</v>
@@ -5248,7 +5248,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/UFWIBTONFRDIAS-UHFFFAOYSA-N</v>
       </c>
       <c r="B104" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C104" t="str">
         <v>null</v>
@@ -5295,7 +5295,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/UGFAIRIUMAVXCW-UHFFFAOYSA-N</v>
       </c>
       <c r="B105" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C105" t="str">
         <v>null</v>
@@ -5342,7 +5342,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/UHOVQNZJYSORNB-UHFFFAOYSA-N</v>
       </c>
       <c r="B106" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C106" t="str">
         <v>null</v>
@@ -5389,7 +5389,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/UOCLXMDMGBRAIB-UHFFFAOYSA-N</v>
       </c>
       <c r="B107" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C107" t="str">
         <v>null</v>
@@ -5436,7 +5436,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/UZUFPBIDKMEQEQ-UHFFFAOYSA-N</v>
       </c>
       <c r="B108" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C108" t="str">
         <v>null</v>
@@ -5483,7 +5483,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/VAYGXNSJCAHWJZ-UHFFFAOYSA-N</v>
       </c>
       <c r="B109" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C109" t="str">
         <v>null</v>
@@ -5530,7 +5530,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/VEZCTZWLJYWARH-UHFFFAOYSA-N</v>
       </c>
       <c r="B110" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C110" t="str">
         <v>null</v>
@@ -5577,7 +5577,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/VHHHONWQHHHLTI-UHFFFAOYSA-N</v>
       </c>
       <c r="B111" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C111" t="str">
         <v>null</v>
@@ -5624,7 +5624,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/VIONGDJUYAYOPU-UHFFFAOYSA-N</v>
       </c>
       <c r="B112" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C112" t="str">
         <v>null</v>
@@ -5671,7 +5671,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/VOWAEIGWURALJQ-UHFFFAOYSA-N</v>
       </c>
       <c r="B113" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C113" t="str">
         <v>null</v>
@@ -5718,7 +5718,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/VOZKAJLKRJDJLL-UHFFFAOYSA-N</v>
       </c>
       <c r="B114" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C114" t="str">
         <v>null</v>
@@ -5765,7 +5765,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/VYZAHLCBVHPDDF-UHFFFAOYSA-N</v>
       </c>
       <c r="B115" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C115" t="str">
         <v>null</v>
@@ -5812,7 +5812,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/VZGDMQKNWNREIO-UHFFFAOYSA-N</v>
       </c>
       <c r="B116" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C116" t="str">
         <v>null</v>
@@ -5859,7 +5859,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WABPQHHGFIMREM-UHFFFAOYSA-N</v>
       </c>
       <c r="B117" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C117" t="str">
         <v>null</v>
@@ -5906,7 +5906,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WBEJYOJJBDISQU-UHFFFAOYSA-N</v>
       </c>
       <c r="B118" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C118" t="str">
         <v>null</v>
@@ -5953,7 +5953,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WCLNVRQZUKYVAI-UHFFFAOYSA-N</v>
       </c>
       <c r="B119" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C119" t="str">
         <v>null</v>
@@ -6000,7 +6000,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WCYYQNSQJHPVMG-UHFFFAOYSA-N</v>
       </c>
       <c r="B120" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C120" t="str">
         <v>null</v>
@@ -6047,7 +6047,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WDECIBYCCFPHNR-UHFFFAOYSA-N</v>
       </c>
       <c r="B121" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C121" t="str">
         <v>null</v>
@@ -6094,7 +6094,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WDMKCPIVJOGHBF-UHFFFAOYSA-N</v>
       </c>
       <c r="B122" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C122" t="str">
         <v>null</v>
@@ -6141,7 +6141,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WJNRPILHGGKWCK-UHFFFAOYSA-N</v>
       </c>
       <c r="B123" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C123" t="str">
         <v>null</v>
@@ -6188,7 +6188,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WLZRMCYVCSSEQC-UHFFFAOYSA-N</v>
       </c>
       <c r="B124" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C124" t="str">
         <v>null</v>
@@ -6235,7 +6235,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WMOVHXAZOJBABW-UHFFFAOYSA-N</v>
       </c>
       <c r="B125" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C125" t="str">
         <v>null</v>
@@ -6282,7 +6282,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WRPIRSINYZBGPK-UHFFFAOYSA-N</v>
       </c>
       <c r="B126" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C126" t="str">
         <v>null</v>
@@ -6329,7 +6329,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WSFSSNUMVMOOMR-UHFFFAOYSA-N</v>
       </c>
       <c r="B127" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C127" t="str">
         <v>null</v>
@@ -6376,7 +6376,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/WSLDOOZREJYCGB-UHFFFAOYSA-N</v>
       </c>
       <c r="B128" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C128" t="str">
         <v>null</v>
@@ -6423,7 +6423,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/XCSGPAVHZFQHGE-UHFFFAOYSA-N</v>
       </c>
       <c r="B129" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C129" t="str">
         <v>null</v>
@@ -6470,7 +6470,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/XKJMBINCVNINCA-UHFFFAOYSA-N</v>
       </c>
       <c r="B130" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C130" t="str">
         <v>null</v>
@@ -6564,7 +6564,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/XMTQQYYKAHVGBJ-UHFFFAOYSA-N</v>
       </c>
       <c r="B132" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C132" t="str">
         <v>null</v>
@@ -6611,7 +6611,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/XNWFRZJHXBZDAG-UHFFFAOYSA-N</v>
       </c>
       <c r="B133" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C133" t="str">
         <v>null</v>
@@ -6658,7 +6658,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/XSTXAVWGXDQKEL-UHFFFAOYSA-N</v>
       </c>
       <c r="B134" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C134" t="str">
         <v>null</v>
@@ -6705,7 +6705,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/XTAHLACQOVXINQ-UHFFFAOYSA-N</v>
       </c>
       <c r="B135" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C135" t="str">
         <v>null</v>
@@ -6752,7 +6752,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/YACLQRRMGMJLJV-UHFFFAOYSA-N</v>
       </c>
       <c r="B136" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C136" t="str">
         <v>null</v>
@@ -6799,7 +6799,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/YBRVSVVVWCFQMG-UHFFFAOYSA-N</v>
       </c>
       <c r="B137" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C137" t="str">
         <v>null</v>
@@ -6846,7 +6846,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/YCLUIPQDHHPDJJ-UHFFFAOYSA-N</v>
       </c>
       <c r="B138" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C138" t="str">
         <v>null</v>
@@ -6893,7 +6893,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/YMWUJEATGCHHMB-UHFFFAOYSA-N</v>
       </c>
       <c r="B139" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C139" t="str">
         <v>null</v>
@@ -6940,7 +6940,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/YNPNZTXNASCQKK-UHFFFAOYSA-N</v>
       </c>
       <c r="B140" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C140" t="str">
         <v>null</v>
@@ -6987,7 +6987,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/YXFVVABEGXRONW-UHFFFAOYSA-N</v>
       </c>
       <c r="B141" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C141" t="str">
         <v>null</v>
@@ -7034,7 +7034,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/ZAFNJMIOTHYJRJ-UHFFFAOYSA-N</v>
       </c>
       <c r="B142" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C142" t="str">
         <v>null</v>
@@ -7081,7 +7081,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/ZMXDDKWLCZADIW-UHFFFAOYSA-N</v>
       </c>
       <c r="B143" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C143" t="str">
         <v>null</v>
@@ -7128,7 +7128,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/ZNQVEEAIQZEUHB-UHFFFAOYSA-N</v>
       </c>
       <c r="B144" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C144" t="str">
         <v>null</v>
@@ -7175,7 +7175,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/ZPQOPVIELGIULI-UHFFFAOYSA-N</v>
       </c>
       <c r="B145" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C145" t="str">
         <v>null</v>
@@ -7222,7 +7222,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/ZVFDTKUVRCTHQE-UHFFFAOYSA-N</v>
       </c>
       <c r="B146" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C146" t="str">
         <v>null</v>
@@ -7269,7 +7269,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/chemische_stof/ZXFXBSWRVIQKOD-UHFFFAOYSA-N</v>
       </c>
       <c r="B147" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://dbpedia.org/ontology/Biomolecule|http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C147" t="str">
         <v>null</v>

</xml_diff>